<commit_message>
improved configuration, tweaked UI for some views
</commit_message>
<xml_diff>
--- a/app1.xlsx
+++ b/app1.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="306">
   <si>
     <t xml:space="preserve">status</t>
   </si>
@@ -840,6 +840,9 @@
     <t xml:space="preserve">Value</t>
   </si>
   <si>
+    <t xml:space="preserve">UsedIn</t>
+  </si>
+  <si>
     <t xml:space="preserve">Comment</t>
   </si>
   <si>
@@ -849,7 +852,10 @@
     <t xml:space="preserve">postgresql</t>
   </si>
   <si>
-    <t xml:space="preserve">could be mysql or other</t>
+    <t xml:space="preserve">config/database.yml</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Some day, could be mysql or other</t>
   </si>
   <si>
     <t xml:space="preserve">host</t>
@@ -861,13 +867,16 @@
     <t xml:space="preserve">could be your ip address</t>
   </si>
   <si>
-    <t xml:space="preserve">database</t>
+    <t xml:space="preserve">database_name</t>
   </si>
   <si>
     <t xml:space="preserve">development</t>
   </si>
   <si>
-    <t xml:space="preserve">username</t>
+    <t xml:space="preserve">Some day, could also create test and production </t>
+  </si>
+  <si>
+    <t xml:space="preserve">database_username</t>
   </si>
   <si>
     <t xml:space="preserve">blog_role</t>
@@ -876,28 +885,80 @@
     <t xml:space="preserve">Database login, must be set up in database prior to running script</t>
   </si>
   <si>
+    <t xml:space="preserve">database_password</t>
+  </si>
+  <si>
     <t xml:space="preserve">  “      needs create database privileges</t>
   </si>
   <si>
-    <t xml:space="preserve">app_admin_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">how the super admin will log into the web app</t>
-  </si>
-  <si>
-    <t xml:space="preserve">app_admin_password</t>
+    <t xml:space="preserve">user_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rails.application.secrets.mail_username</t>
+  </si>
+  <si>
+    <t xml:space="preserve">config/environments/development.rb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">credentials for mail server, not automatically used right now</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rails.application.secrets.mail_password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   “</t>
+  </si>
+  <si>
+    <t xml:space="preserve">domain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">smtp.gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">port</t>
+  </si>
+  <si>
+    <t xml:space="preserve">authentication</t>
+  </si>
+  <si>
+    <t xml:space="preserve">plain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">enable_starttls_auto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mail_username</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sparton.clinic1@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">config/secrets.yml</t>
+  </si>
+  <si>
+    <t xml:space="preserve">email (and other apps) will fish secrets from here. Should not be put into VCS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mail_password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">terces123</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
+  <numFmts count="6">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="M/D/YYYY"/>
     <numFmt numFmtId="166" formatCode="MM/DD/YYYY"/>
     <numFmt numFmtId="167" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
     <numFmt numFmtId="168" formatCode="MM/DD/YYYY\ HH:MM:SS"/>
+    <numFmt numFmtId="169" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
   <fonts count="8">
     <font>
@@ -998,7 +1059,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1079,11 +1140,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1173,9 +1242,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="9.78947368421053"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.8947368421053"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.78947368421053"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="9.91093117408907"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.2591093117409"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.91093117408907"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1245,13 +1314,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="25.9514170040486"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="22.8947368421053"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="20.6882591093117"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.5668016194332"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="33.1781376518219"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="24.2388663967611"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.4251012145749"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="26.5668016194332"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="23.3805668016194"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="21.1821862348178"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="27.2995951417004"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="33.914979757085"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="24.8502024291498"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.54655870445344"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1686,8 +1755,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="23.6315789473684"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.78947368421053"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="24.1174089068826"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.91093117408907"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1722,7 +1791,7 @@
       </c>
       <c r="C3" s="1" t="n">
         <f aca="true">NOW() +RAND()*1000</f>
-        <v>43212.5809094434</v>
+        <v>42795.6802746477</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1735,7 +1804,7 @@
       </c>
       <c r="C4" s="1" t="n">
         <f aca="true">NOW() +RAND()*1000</f>
-        <v>43545.5223033</v>
+        <v>43057.3603312528</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1748,7 +1817,7 @@
       </c>
       <c r="C5" s="1" t="n">
         <f aca="true">NOW() +RAND()*1000</f>
-        <v>43158.8662442794</v>
+        <v>43127.9392892374</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1761,7 +1830,7 @@
       </c>
       <c r="C6" s="1" t="n">
         <f aca="true">NOW() +RAND()*1000</f>
-        <v>42790.3158333455</v>
+        <v>43743.6417006672</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1774,7 +1843,7 @@
       </c>
       <c r="C7" s="1" t="n">
         <f aca="true">NOW() +RAND()*1000</f>
-        <v>43684.9756922602</v>
+        <v>43130.3731738093</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1787,7 +1856,7 @@
       </c>
       <c r="C8" s="1" t="n">
         <f aca="true">NOW() +RAND()*1000</f>
-        <v>43041.8129668896</v>
+        <v>43240.2425823536</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1800,7 +1869,7 @@
       </c>
       <c r="C9" s="1" t="n">
         <f aca="true">NOW() +RAND()*1000</f>
-        <v>43327.4169632939</v>
+        <v>43214.0965490759</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1813,7 +1882,7 @@
       </c>
       <c r="C10" s="1" t="n">
         <f aca="true">NOW() +RAND()*1000</f>
-        <v>43556.4409887449</v>
+        <v>42807.2457316284</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1826,7 +1895,7 @@
       </c>
       <c r="C11" s="1" t="n">
         <f aca="true">NOW() +RAND()*1000</f>
-        <v>43529.0756262013</v>
+        <v>42829.0594259154</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1839,7 +1908,7 @@
       </c>
       <c r="C12" s="1" t="n">
         <f aca="true">NOW() +RAND()*1000</f>
-        <v>43135.4908833929</v>
+        <v>42960.7421623302</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1852,7 +1921,7 @@
       </c>
       <c r="C13" s="1" t="n">
         <f aca="true">NOW() +RAND()*1000</f>
-        <v>43666.2183029823</v>
+        <v>43358.5612741858</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1865,7 +1934,7 @@
       </c>
       <c r="C14" s="1" t="n">
         <f aca="true">NOW() +RAND()*1000</f>
-        <v>43671.9161165643</v>
+        <v>42790.5915838549</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1878,7 +1947,7 @@
       </c>
       <c r="C15" s="1" t="n">
         <f aca="true">TODAY()</f>
-        <v>42755</v>
+        <v>42760</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1891,7 +1960,7 @@
       </c>
       <c r="C16" s="1" t="n">
         <f aca="true">TODAY()</f>
-        <v>42755</v>
+        <v>42760</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1904,7 +1973,7 @@
       </c>
       <c r="C17" s="1" t="n">
         <f aca="true">TODAY()</f>
-        <v>42755</v>
+        <v>42760</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1917,7 +1986,7 @@
       </c>
       <c r="C18" s="1" t="n">
         <f aca="true">TODAY()</f>
-        <v>42755</v>
+        <v>42760</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1930,7 +1999,7 @@
       </c>
       <c r="C19" s="1" t="n">
         <f aca="true">TODAY()</f>
-        <v>42755</v>
+        <v>42760</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1943,7 +2012,7 @@
       </c>
       <c r="C20" s="1" t="n">
         <f aca="true">TODAY()</f>
-        <v>42755</v>
+        <v>42760</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1956,7 +2025,7 @@
       </c>
       <c r="C21" s="1" t="n">
         <f aca="true">TODAY()</f>
-        <v>42755</v>
+        <v>42760</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1969,7 +2038,7 @@
       </c>
       <c r="C22" s="1" t="n">
         <f aca="true">TODAY()</f>
-        <v>42755</v>
+        <v>42760</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1982,7 +2051,7 @@
       </c>
       <c r="C23" s="1" t="n">
         <f aca="true">TODAY()</f>
-        <v>42755</v>
+        <v>42760</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1995,7 +2064,7 @@
       </c>
       <c r="C24" s="1" t="n">
         <f aca="true">TODAY()</f>
-        <v>42755</v>
+        <v>42760</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2008,7 +2077,7 @@
       </c>
       <c r="C25" s="1" t="n">
         <f aca="true">TODAY()</f>
-        <v>42755</v>
+        <v>42760</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2021,7 +2090,7 @@
       </c>
       <c r="C26" s="1" t="n">
         <f aca="true">TODAY()</f>
-        <v>42755</v>
+        <v>42760</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2034,7 +2103,7 @@
       </c>
       <c r="C27" s="1" t="n">
         <f aca="true">TODAY()</f>
-        <v>42755</v>
+        <v>42760</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2047,7 +2116,7 @@
       </c>
       <c r="C28" s="1" t="n">
         <f aca="true">TODAY()</f>
-        <v>42755</v>
+        <v>42760</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2060,7 +2129,7 @@
       </c>
       <c r="C29" s="1" t="n">
         <f aca="true">TODAY()</f>
-        <v>42755</v>
+        <v>42760</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2073,7 +2142,7 @@
       </c>
       <c r="C30" s="1" t="n">
         <f aca="true">TODAY()</f>
-        <v>42755</v>
+        <v>42760</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2086,7 +2155,7 @@
       </c>
       <c r="C31" s="1" t="n">
         <f aca="true">TODAY()</f>
-        <v>42755</v>
+        <v>42760</v>
       </c>
     </row>
   </sheetData>
@@ -2113,12 +2182,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="9.78947368421053"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.0364372469636"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.5465587044534"/>
-    <col collapsed="false" hidden="false" max="8" min="6" style="0" width="9.78947368421053"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="20.6882591093117"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="9.78947368421053"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="9.91093117408907"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.5222672064777"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.0364372469636"/>
+    <col collapsed="false" hidden="false" max="8" min="6" style="0" width="9.91093117408907"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="21.1821862348178"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="9.91093117408907"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2211,11 +2280,11 @@
       </c>
       <c r="F3" s="3" t="n">
         <f aca="true">ROUND(RAND()*15+30,3)</f>
-        <v>43.214</v>
+        <v>33.964</v>
       </c>
       <c r="G3" s="3" t="n">
         <f aca="true">ROUND(-(RAND()*40+80),3)</f>
-        <v>-80.453</v>
+        <v>-88.073</v>
       </c>
       <c r="H3" s="3" t="str">
         <f aca="false">CONCATENATE(DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)))</f>
@@ -2223,7 +2292,7 @@
       </c>
       <c r="I3" s="5" t="n">
         <f aca="true">NOW()+100 + RAND()*365</f>
-        <v>43050.7883589601</v>
+        <v>42924.3640982918</v>
       </c>
       <c r="J3" s="3" t="n">
         <f aca="false">RANDBETWEEN(0,1000)</f>
@@ -2255,11 +2324,11 @@
       </c>
       <c r="F4" s="3" t="n">
         <f aca="true">ROUND(RAND()*15+30,3)</f>
-        <v>39.355</v>
+        <v>43.038</v>
       </c>
       <c r="G4" s="3" t="n">
         <f aca="true">ROUND(-(RAND()*40+80),3)</f>
-        <v>-99.846</v>
+        <v>-104.373</v>
       </c>
       <c r="H4" s="3" t="str">
         <f aca="false">CONCATENATE(DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)))</f>
@@ -2267,7 +2336,7 @@
       </c>
       <c r="I4" s="5" t="n">
         <f aca="true">NOW()+100 + RAND()*365</f>
-        <v>43170.2430807717</v>
+        <v>43188.0087600524</v>
       </c>
       <c r="J4" s="3" t="n">
         <f aca="false">RANDBETWEEN(0,1000)</f>
@@ -2299,11 +2368,11 @@
       </c>
       <c r="F5" s="3" t="n">
         <f aca="true">ROUND(RAND()*15+30,3)</f>
-        <v>30.906</v>
+        <v>37.474</v>
       </c>
       <c r="G5" s="3" t="n">
         <f aca="true">ROUND(-(RAND()*40+80),3)</f>
-        <v>-113.632</v>
+        <v>-119.643</v>
       </c>
       <c r="H5" s="3" t="str">
         <f aca="false">CONCATENATE(DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)))</f>
@@ -2311,7 +2380,7 @@
       </c>
       <c r="I5" s="5" t="n">
         <f aca="true">NOW()+100 + RAND()*365</f>
-        <v>43159.3156161525</v>
+        <v>42978.1741543979</v>
       </c>
       <c r="J5" s="3" t="n">
         <f aca="false">RANDBETWEEN(0,1000)</f>
@@ -2343,11 +2412,11 @@
       </c>
       <c r="F6" s="3" t="n">
         <f aca="true">ROUND(RAND()*15+30,3)</f>
-        <v>39.902</v>
+        <v>34.008</v>
       </c>
       <c r="G6" s="3" t="n">
         <f aca="true">ROUND(-(RAND()*40+80),3)</f>
-        <v>-98.427</v>
+        <v>-82.049</v>
       </c>
       <c r="H6" s="3" t="str">
         <f aca="false">CONCATENATE(DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)))</f>
@@ -2355,7 +2424,7 @@
       </c>
       <c r="I6" s="5" t="n">
         <f aca="true">NOW()+100 + RAND()*365</f>
-        <v>42884.4121236989</v>
+        <v>43016.7329581767</v>
       </c>
       <c r="J6" s="3" t="n">
         <f aca="false">RANDBETWEEN(0,1000)</f>
@@ -2387,11 +2456,11 @@
       </c>
       <c r="F7" s="3" t="n">
         <f aca="true">ROUND(RAND()*15+30,3)</f>
-        <v>43.568</v>
+        <v>42.887</v>
       </c>
       <c r="G7" s="3" t="n">
         <f aca="true">ROUND(-(RAND()*40+80),3)</f>
-        <v>-112.986</v>
+        <v>-95.673</v>
       </c>
       <c r="H7" s="3" t="str">
         <f aca="false">CONCATENATE(DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)))</f>
@@ -2399,7 +2468,7 @@
       </c>
       <c r="I7" s="5" t="n">
         <f aca="true">NOW()+100 + RAND()*365</f>
-        <v>42950.8723081282</v>
+        <v>43019.5173244928</v>
       </c>
       <c r="J7" s="3" t="n">
         <f aca="false">RANDBETWEEN(0,1000)</f>
@@ -2431,11 +2500,11 @@
       </c>
       <c r="F8" s="3" t="n">
         <f aca="true">ROUND(RAND()*15+30,3)</f>
-        <v>36.487</v>
+        <v>30.582</v>
       </c>
       <c r="G8" s="3" t="n">
         <f aca="true">ROUND(-(RAND()*40+80),3)</f>
-        <v>-111.934</v>
+        <v>-119.424</v>
       </c>
       <c r="H8" s="3" t="str">
         <f aca="false">CONCATENATE(DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)))</f>
@@ -2443,7 +2512,7 @@
       </c>
       <c r="I8" s="5" t="n">
         <f aca="true">NOW()+100 + RAND()*365</f>
-        <v>43016.9110783804</v>
+        <v>43135.3109004055</v>
       </c>
       <c r="J8" s="3" t="n">
         <f aca="false">RANDBETWEEN(0,1000)</f>
@@ -2475,11 +2544,11 @@
       </c>
       <c r="F9" s="3" t="n">
         <f aca="true">ROUND(RAND()*15+30,3)</f>
-        <v>37.803</v>
+        <v>39.814</v>
       </c>
       <c r="G9" s="3" t="n">
         <f aca="true">ROUND(-(RAND()*40+80),3)</f>
-        <v>-97.569</v>
+        <v>-100.306</v>
       </c>
       <c r="H9" s="3" t="str">
         <f aca="false">CONCATENATE(DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)))</f>
@@ -2487,7 +2556,7 @@
       </c>
       <c r="I9" s="5" t="n">
         <f aca="true">NOW()+100 + RAND()*365</f>
-        <v>43117.2365391687</v>
+        <v>43163.6342589653</v>
       </c>
       <c r="J9" s="3" t="n">
         <f aca="false">RANDBETWEEN(0,1000)</f>
@@ -2519,11 +2588,11 @@
       </c>
       <c r="F10" s="3" t="n">
         <f aca="true">ROUND(RAND()*15+30,3)</f>
-        <v>42.359</v>
+        <v>38.514</v>
       </c>
       <c r="G10" s="3" t="n">
         <f aca="true">ROUND(-(RAND()*40+80),3)</f>
-        <v>-117.725</v>
+        <v>-104.27</v>
       </c>
       <c r="H10" s="3" t="str">
         <f aca="false">CONCATENATE(DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)))</f>
@@ -2531,7 +2600,7 @@
       </c>
       <c r="I10" s="5" t="n">
         <f aca="true">NOW()+100 + RAND()*365</f>
-        <v>42956.5160013738</v>
+        <v>43042.154874953</v>
       </c>
       <c r="J10" s="3" t="n">
         <f aca="false">RANDBETWEEN(0,1000)</f>
@@ -2563,11 +2632,11 @@
       </c>
       <c r="F11" s="3" t="n">
         <f aca="true">ROUND(RAND()*15+30,3)</f>
-        <v>32.228</v>
+        <v>40.53</v>
       </c>
       <c r="G11" s="3" t="n">
         <f aca="true">ROUND(-(RAND()*40+80),3)</f>
-        <v>-93.54</v>
+        <v>-103.404</v>
       </c>
       <c r="H11" s="3" t="str">
         <f aca="false">CONCATENATE(DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)))</f>
@@ -2575,7 +2644,7 @@
       </c>
       <c r="I11" s="5" t="n">
         <f aca="true">NOW()+100 + RAND()*365</f>
-        <v>42986.5848303066</v>
+        <v>42885.675928022</v>
       </c>
       <c r="J11" s="3" t="n">
         <f aca="false">RANDBETWEEN(0,1000)</f>
@@ -2607,11 +2676,11 @@
       </c>
       <c r="F12" s="3" t="n">
         <f aca="true">ROUND(RAND()*15+30,3)</f>
-        <v>43.893</v>
+        <v>37.023</v>
       </c>
       <c r="G12" s="3" t="n">
         <f aca="true">ROUND(-(RAND()*40+80),3)</f>
-        <v>-104.851</v>
+        <v>-82.759</v>
       </c>
       <c r="H12" s="3" t="str">
         <f aca="false">CONCATENATE(DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)))</f>
@@ -2619,7 +2688,7 @@
       </c>
       <c r="I12" s="5" t="n">
         <f aca="true">NOW()+100 + RAND()*365</f>
-        <v>43181.5446642436</v>
+        <v>43196.2555472522</v>
       </c>
       <c r="J12" s="3" t="n">
         <f aca="false">RANDBETWEEN(0,1000)</f>
@@ -2651,11 +2720,11 @@
       </c>
       <c r="F13" s="3" t="n">
         <f aca="true">ROUND(RAND()*15+30,3)</f>
-        <v>44.204</v>
+        <v>43.096</v>
       </c>
       <c r="G13" s="3" t="n">
         <f aca="true">ROUND(-(RAND()*40+80),3)</f>
-        <v>-104.674</v>
+        <v>-93.079</v>
       </c>
       <c r="H13" s="3" t="str">
         <f aca="false">CONCATENATE(DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)))</f>
@@ -2663,7 +2732,7 @@
       </c>
       <c r="I13" s="5" t="n">
         <f aca="true">NOW()+100 + RAND()*365</f>
-        <v>43011.2346258283</v>
+        <v>42906.456119578</v>
       </c>
       <c r="J13" s="3" t="n">
         <f aca="false">RANDBETWEEN(0,1000)</f>
@@ -2731,14 +2800,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="6" width="9.78947368421053"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="6" width="25.82995951417"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="6" width="11.9959514170041"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="6" width="9.78947368421053"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.4048582995951"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.78947368421053"/>
-    <col collapsed="false" hidden="false" max="12" min="7" style="6" width="16.8947368421053"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="9.78947368421053"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="6" width="9.91093117408907"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="6" width="26.4453441295547"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="6" width="12.2388663967611"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="6" width="9.91093117408907"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.5263157894737"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.91093117408907"/>
+    <col collapsed="false" hidden="false" max="12" min="7" style="6" width="17.2591093117409"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="9.91093117408907"/>
   </cols>
   <sheetData>
     <row r="1" s="8" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4150,9 +4219,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="9.78947368421053"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.4251012145749"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.78947368421053"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="9.91093117408907"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.668016194332"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.91093117408907"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4217,7 +4286,7 @@
       </c>
       <c r="C3" s="12" t="n">
         <f aca="true">NOW()-90*365*RAND()</f>
-        <v>39775.207877739</v>
+        <v>39501.3414031615</v>
       </c>
       <c r="D3" s="0" t="s">
         <v>175</v>
@@ -4247,7 +4316,7 @@
       </c>
       <c r="C4" s="12" t="n">
         <f aca="true">NOW()-90*365*RAND()</f>
-        <v>10247.4740518046</v>
+        <v>16843.4421976712</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>175</v>
@@ -4277,7 +4346,7 @@
       </c>
       <c r="C5" s="12" t="n">
         <f aca="true">NOW()-90*365*RAND()</f>
-        <v>21788.2860849428</v>
+        <v>21589.2368559503</v>
       </c>
       <c r="D5" s="0" t="s">
         <v>175</v>
@@ -4307,7 +4376,7 @@
       </c>
       <c r="C6" s="12" t="n">
         <f aca="true">NOW()-90*365*RAND()</f>
-        <v>25392.4437426164</v>
+        <v>40296.7035861034</v>
       </c>
       <c r="D6" s="0" t="s">
         <v>175</v>
@@ -4337,7 +4406,7 @@
       </c>
       <c r="C7" s="12" t="n">
         <f aca="true">NOW()-90*365*RAND()</f>
-        <v>37019.5141304948</v>
+        <v>39629.931569851</v>
       </c>
       <c r="D7" s="0" t="s">
         <v>175</v>
@@ -4367,7 +4436,7 @@
       </c>
       <c r="C8" s="12" t="n">
         <f aca="true">NOW()-90*365*RAND()</f>
-        <v>23030.9059321257</v>
+        <v>31779.8979278321</v>
       </c>
       <c r="D8" s="0" t="s">
         <v>175</v>
@@ -4397,7 +4466,7 @@
       </c>
       <c r="C9" s="12" t="n">
         <f aca="true">NOW()-90*365*RAND()</f>
-        <v>25376.3575476065</v>
+        <v>37302.381040631</v>
       </c>
       <c r="D9" s="0" t="s">
         <v>175</v>
@@ -4427,7 +4496,7 @@
       </c>
       <c r="C10" s="12" t="n">
         <f aca="true">NOW()-90*365*RAND()</f>
-        <v>38297.5436083537</v>
+        <v>22902.0111697759</v>
       </c>
       <c r="D10" s="0" t="s">
         <v>175</v>
@@ -4457,7 +4526,7 @@
       </c>
       <c r="C11" s="12" t="n">
         <f aca="true">NOW()-90*365*RAND()</f>
-        <v>12269.1799538849</v>
+        <v>35348.9109630396</v>
       </c>
       <c r="D11" s="0" t="s">
         <v>175</v>
@@ -4487,7 +4556,7 @@
       </c>
       <c r="C12" s="12" t="n">
         <f aca="true">NOW()-90*365*RAND()</f>
-        <v>42664.3215446216</v>
+        <v>10753.9436332744</v>
       </c>
       <c r="D12" s="0" t="s">
         <v>175</v>
@@ -4517,7 +4586,7 @@
       </c>
       <c r="C13" s="12" t="n">
         <f aca="true">NOW()-90*365*RAND()</f>
-        <v>23456.9147372753</v>
+        <v>31957.2587588869</v>
       </c>
       <c r="D13" s="0" t="s">
         <v>175</v>
@@ -4547,7 +4616,7 @@
       </c>
       <c r="C14" s="12" t="n">
         <f aca="true">NOW()-90*365*RAND()</f>
-        <v>27512.9577934871</v>
+        <v>21104.7958335609</v>
       </c>
       <c r="D14" s="0" t="s">
         <v>196</v>
@@ -4577,7 +4646,7 @@
       </c>
       <c r="C15" s="12" t="n">
         <f aca="true">NOW()-90*365*RAND()</f>
-        <v>33550.5735512863</v>
+        <v>11527.5258166523</v>
       </c>
       <c r="D15" s="0" t="s">
         <v>196</v>
@@ -4607,7 +4676,7 @@
       </c>
       <c r="C16" s="12" t="n">
         <f aca="true">NOW()-90*365*RAND()</f>
-        <v>32851.9518937586</v>
+        <v>11655.6557118445</v>
       </c>
       <c r="D16" s="0" t="s">
         <v>196</v>
@@ -4637,7 +4706,7 @@
       </c>
       <c r="C17" s="12" t="n">
         <f aca="true">NOW()-90*365*RAND()</f>
-        <v>12923.6084256194</v>
+        <v>28414.3802652895</v>
       </c>
       <c r="D17" s="0" t="s">
         <v>196</v>
@@ -4667,7 +4736,7 @@
       </c>
       <c r="C18" s="12" t="n">
         <f aca="true">NOW()-90*365*RAND()</f>
-        <v>32152.0539834419</v>
+        <v>29591.977886474</v>
       </c>
       <c r="D18" s="0" t="s">
         <v>196</v>
@@ -4697,7 +4766,7 @@
       </c>
       <c r="C19" s="12" t="n">
         <f aca="true">NOW()-90*365*RAND()</f>
-        <v>18345.1412830965</v>
+        <v>33342.0815425449</v>
       </c>
       <c r="D19" s="0" t="s">
         <v>196</v>
@@ -4727,7 +4796,7 @@
       </c>
       <c r="C20" s="12" t="n">
         <f aca="true">NOW()-90*365*RAND()</f>
-        <v>24190.2889408012</v>
+        <v>36508.8843419367</v>
       </c>
       <c r="D20" s="0" t="s">
         <v>196</v>
@@ -4757,7 +4826,7 @@
       </c>
       <c r="C21" s="12" t="n">
         <f aca="true">NOW()-90*365*RAND()</f>
-        <v>17060.0782099594</v>
+        <v>26560.5731057971</v>
       </c>
       <c r="D21" s="0" t="s">
         <v>196</v>
@@ -4787,7 +4856,7 @@
       </c>
       <c r="C22" s="12" t="n">
         <f aca="true">NOW()-90*365*RAND()</f>
-        <v>32883.1955790694</v>
+        <v>16116.583948489</v>
       </c>
       <c r="D22" s="0" t="s">
         <v>196</v>
@@ -4831,10 +4900,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="7" min="1" style="6" width="9.66801619433198"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="13" width="23.8744939271255"/>
-    <col collapsed="false" hidden="false" max="13" min="9" style="0" width="23.8744939271255"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="9.78947368421053"/>
+    <col collapsed="false" hidden="false" max="7" min="1" style="6" width="9.78947368421053"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="13" width="24.3603238866397"/>
+    <col collapsed="false" hidden="false" max="13" min="9" style="0" width="24.3603238866397"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="9.91093117408907"/>
   </cols>
   <sheetData>
     <row r="1" s="16" customFormat="true" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4925,7 +4994,7 @@
       </c>
       <c r="H3" s="17" t="n">
         <f aca="true">NOW() -RAND()*99.7</f>
-        <v>42723.6891987837</v>
+        <v>42743.1902499568</v>
       </c>
       <c r="I3" s="0" t="s">
         <v>222</v>
@@ -4961,7 +5030,7 @@
       </c>
       <c r="H4" s="17" t="n">
         <f aca="true">NOW() -RAND()*100</f>
-        <v>42713.1407347243</v>
+        <v>42736.3535385482</v>
       </c>
       <c r="I4" s="0" t="s">
         <v>223</v>
@@ -4999,7 +5068,7 @@
       </c>
       <c r="H5" s="17" t="n">
         <f aca="true">NOW() -RAND()*100</f>
-        <v>42682.2765693108</v>
+        <v>42709.4845487654</v>
       </c>
       <c r="I5" s="0" t="s">
         <v>224</v>
@@ -5037,7 +5106,7 @@
       </c>
       <c r="H6" s="17" t="n">
         <f aca="true">NOW() -RAND()*100</f>
-        <v>42698.7518229751</v>
+        <v>42672.3532023695</v>
       </c>
       <c r="I6" s="0" t="s">
         <v>225</v>
@@ -5075,7 +5144,7 @@
       </c>
       <c r="H7" s="17" t="n">
         <f aca="true">NOW() -RAND()*100</f>
-        <v>42656.8748782841</v>
+        <v>42745.8495281464</v>
       </c>
       <c r="I7" s="0" t="s">
         <v>226</v>
@@ -5113,7 +5182,7 @@
       </c>
       <c r="H8" s="17" t="n">
         <f aca="true">NOW() -RAND()*100</f>
-        <v>42742.4803643381</v>
+        <v>42700.3469847428</v>
       </c>
       <c r="I8" s="0" t="s">
         <v>227</v>
@@ -5151,7 +5220,7 @@
       </c>
       <c r="H9" s="17" t="n">
         <f aca="true">NOW() -RAND()*100</f>
-        <v>42674.7581719724</v>
+        <v>42745.7254026287</v>
       </c>
       <c r="I9" s="0" t="s">
         <v>228</v>
@@ -5189,7 +5258,7 @@
       </c>
       <c r="H10" s="17" t="n">
         <f aca="true">NOW() -RAND()*100</f>
-        <v>42754.6908006496</v>
+        <v>42665.0375584331</v>
       </c>
       <c r="I10" s="0" t="s">
         <v>229</v>
@@ -5227,7 +5296,7 @@
       </c>
       <c r="H11" s="17" t="n">
         <f aca="true">NOW() -RAND()*100</f>
-        <v>42683.9561998356</v>
+        <v>42740.6957093297</v>
       </c>
       <c r="I11" s="0" t="s">
         <v>230</v>
@@ -5265,7 +5334,7 @@
       </c>
       <c r="H12" s="17" t="n">
         <f aca="true">NOW() -RAND()*100</f>
-        <v>42740.8688985807</v>
+        <v>42737.9709746287</v>
       </c>
       <c r="I12" s="0" t="s">
         <v>231</v>
@@ -5303,7 +5372,7 @@
       </c>
       <c r="H13" s="17" t="n">
         <f aca="true">NOW() -RAND()*100</f>
-        <v>42665.3457921612</v>
+        <v>42710.0690547679</v>
       </c>
       <c r="I13" s="0" t="s">
         <v>232</v>
@@ -5341,7 +5410,7 @@
       </c>
       <c r="H14" s="17" t="n">
         <f aca="true">NOW() -RAND()*100</f>
-        <v>42658.8545524769</v>
+        <v>42716.0171368997</v>
       </c>
       <c r="I14" s="0" t="s">
         <v>233</v>
@@ -5379,7 +5448,7 @@
       </c>
       <c r="H15" s="17" t="n">
         <f aca="true">NOW() -RAND()*100</f>
-        <v>42736.4436902852</v>
+        <v>42674.7783471665</v>
       </c>
       <c r="I15" s="0" t="s">
         <v>234</v>
@@ -5417,7 +5486,7 @@
       </c>
       <c r="H16" s="17" t="n">
         <f aca="true">NOW() -RAND()*100</f>
-        <v>42678.7856624411</v>
+        <v>42722.8316821317</v>
       </c>
       <c r="I16" s="0" t="s">
         <v>235</v>
@@ -5455,7 +5524,7 @@
       </c>
       <c r="H17" s="17" t="n">
         <f aca="true">NOW() -RAND()*100</f>
-        <v>42679.4634066311</v>
+        <v>42757.1599649736</v>
       </c>
       <c r="I17" s="0" t="s">
         <v>236</v>
@@ -5493,7 +5562,7 @@
       </c>
       <c r="H18" s="17" t="n">
         <f aca="true">NOW() -RAND()*100</f>
-        <v>42657.3990312735</v>
+        <v>42679.0609330361</v>
       </c>
       <c r="I18" s="0" t="s">
         <v>237</v>
@@ -5531,7 +5600,7 @@
       </c>
       <c r="H19" s="17" t="n">
         <f aca="true">NOW() -RAND()*100</f>
-        <v>42699.6300553981</v>
+        <v>42674.6825612462</v>
       </c>
       <c r="I19" s="0" t="s">
         <v>238</v>
@@ -5569,7 +5638,7 @@
       </c>
       <c r="H20" s="17" t="n">
         <f aca="true">NOW() -RAND()*100</f>
-        <v>42659.9993265992</v>
+        <v>42731.8205698679</v>
       </c>
       <c r="I20" s="0" t="s">
         <v>239</v>
@@ -5607,7 +5676,7 @@
       </c>
       <c r="H21" s="17" t="n">
         <f aca="true">NOW() -RAND()*100</f>
-        <v>42754.9951909326</v>
+        <v>42696.5219224288</v>
       </c>
       <c r="I21" s="0" t="s">
         <v>240</v>
@@ -5645,7 +5714,7 @@
       </c>
       <c r="H22" s="17" t="n">
         <f aca="true">NOW() -RAND()*100</f>
-        <v>42716.4016980217</v>
+        <v>42682.4390475461</v>
       </c>
       <c r="I22" s="0" t="s">
         <v>241</v>
@@ -5683,7 +5752,7 @@
       </c>
       <c r="H23" s="17" t="n">
         <f aca="true">NOW() -RAND()*100</f>
-        <v>42738.2341130915</v>
+        <v>42700.7478095004</v>
       </c>
       <c r="I23" s="0" t="s">
         <v>242</v>
@@ -5721,7 +5790,7 @@
       </c>
       <c r="H24" s="17" t="n">
         <f aca="true">NOW() -RAND()*100</f>
-        <v>42693.7130612852</v>
+        <v>42687.6765431392</v>
       </c>
       <c r="I24" s="0" t="s">
         <v>243</v>
@@ -5759,7 +5828,7 @@
       </c>
       <c r="H25" s="17" t="n">
         <f aca="true">NOW() -RAND()*100</f>
-        <v>42669.1265946903</v>
+        <v>42740.2206678902</v>
       </c>
       <c r="I25" s="0" t="s">
         <v>244</v>
@@ -5797,7 +5866,7 @@
       </c>
       <c r="H26" s="17" t="n">
         <f aca="true">NOW() -RAND()*100</f>
-        <v>42693.175357516</v>
+        <v>42738.5250510615</v>
       </c>
       <c r="I26" s="0" t="s">
         <v>245</v>
@@ -5835,7 +5904,7 @@
       </c>
       <c r="H27" s="17" t="n">
         <f aca="true">NOW() -RAND()*100</f>
-        <v>42748.1961901762</v>
+        <v>42760.6308758008</v>
       </c>
       <c r="I27" s="0" t="s">
         <v>246</v>
@@ -5873,7 +5942,7 @@
       </c>
       <c r="H28" s="17" t="n">
         <f aca="true">NOW() -RAND()*100</f>
-        <v>42672.2244881388</v>
+        <v>42710.4316849075</v>
       </c>
       <c r="I28" s="0" t="s">
         <v>247</v>
@@ -5911,7 +5980,7 @@
       </c>
       <c r="H29" s="17" t="n">
         <f aca="true">NOW() -RAND()*100</f>
-        <v>42689.9992655369</v>
+        <v>42749.0461795868</v>
       </c>
       <c r="I29" s="0" t="s">
         <v>248</v>
@@ -5949,7 +6018,7 @@
       </c>
       <c r="H30" s="17" t="n">
         <f aca="true">NOW() -RAND()*100</f>
-        <v>42661.2972149472</v>
+        <v>42674.0564125614</v>
       </c>
       <c r="I30" s="0" t="s">
         <v>249</v>
@@ -5987,7 +6056,7 @@
       </c>
       <c r="H31" s="17" t="n">
         <f aca="true">NOW() -RAND()*100</f>
-        <v>42719.7713783271</v>
+        <v>42689.4790010351</v>
       </c>
       <c r="I31" s="0" t="s">
         <v>250</v>
@@ -6025,7 +6094,7 @@
       </c>
       <c r="H32" s="17" t="n">
         <f aca="true">NOW() -RAND()*100</f>
-        <v>42738.5287158647</v>
+        <v>42664.8385308753</v>
       </c>
       <c r="I32" s="0" t="s">
         <v>251</v>
@@ -6063,7 +6132,7 @@
       </c>
       <c r="H33" s="17" t="n">
         <f aca="true">NOW() -RAND()*100</f>
-        <v>42659.0462499308</v>
+        <v>42701.7328191303</v>
       </c>
       <c r="I33" s="0" t="s">
         <v>252</v>
@@ -6101,7 +6170,7 @@
       </c>
       <c r="H34" s="17" t="n">
         <f aca="true">NOW() -RAND()*100</f>
-        <v>42672.3450494495</v>
+        <v>42677.9292542771</v>
       </c>
       <c r="I34" s="0" t="s">
         <v>253</v>
@@ -6139,7 +6208,7 @@
       </c>
       <c r="H35" s="17" t="n">
         <f aca="true">NOW() -RAND()*100</f>
-        <v>42658.2715915943</v>
+        <v>42735.8974739042</v>
       </c>
       <c r="I35" s="0" t="s">
         <v>254</v>
@@ -6171,11 +6240,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="18" width="31"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="18" width="13.9838056680162"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="18" width="28.085020242915"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="18" width="11.0688259109312"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="18" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="18" width="31.7085020242915"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="18" width="14.3238866396761"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="18" width="28.7732793522267"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="18" width="11.3846153846154"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="18" width="9.30364372469636"/>
   </cols>
   <sheetData>
     <row r="1" s="19" customFormat="true" ht="14.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6202,6 +6271,7 @@
       <c r="C2" s="16" t="s">
         <v>260</v>
       </c>
+      <c r="D2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="14.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="16" t="s">
@@ -6213,6 +6283,7 @@
       <c r="C3" s="16" t="s">
         <v>261</v>
       </c>
+      <c r="D3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="14.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="16" t="s">
@@ -6224,6 +6295,7 @@
       <c r="C4" s="16" t="s">
         <v>263</v>
       </c>
+      <c r="D4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="14.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="16" t="s">
@@ -6353,103 +6425,234 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C8"/>
+  <dimension ref="1:15"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
+      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.85"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.3805668016194"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.5303643724696"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="56.4089068825911"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="20" width="21.7935222672065"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="20" width="32.6275303643725"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="20" width="34.3765182186235"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="20" width="57.7813765182186"/>
+    <col collapsed="false" hidden="false" max="1023" min="5" style="20" width="9.30364372469636"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="9.30364372469636"/>
   </cols>
   <sheetData>
-    <row r="1" s="20" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="20" t="s">
+    <row r="1" s="21" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="21" t="s">
         <v>268</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="21" t="s">
         <v>269</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="21" t="s">
         <v>270</v>
       </c>
+      <c r="D1" s="21" t="s">
+        <v>271</v>
+      </c>
+      <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>271</v>
-      </c>
-      <c r="B2" s="0" t="s">
+      <c r="A2" s="20" t="s">
         <v>272</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="B2" s="20" t="s">
         <v>273</v>
       </c>
+      <c r="C2" s="20" t="s">
+        <v>274</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>275</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="20" t="s">
+        <v>276</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>277</v>
+      </c>
+      <c r="C3" s="20" t="s">
         <v>274</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>275</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>276</v>
+      <c r="D3" s="20" t="s">
+        <v>278</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>277</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>278</v>
+      <c r="A4" s="20" t="s">
+        <v>279</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>280</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>274</v>
+      </c>
+      <c r="D4" s="22" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>279</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>280</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>281</v>
+      <c r="A5" s="20" t="s">
+        <v>282</v>
+      </c>
+      <c r="B5" s="20" t="s">
+        <v>283</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>274</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="20" t="s">
+        <v>285</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>283</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>274</v>
+      </c>
+      <c r="D6" s="20" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="20" t="s">
+        <v>287</v>
+      </c>
+      <c r="B7" s="20" t="s">
+        <v>288</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>289</v>
+      </c>
+      <c r="D7" s="20" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="B6" s="0" t="s">
-        <v>280</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>283</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>121</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>285</v>
-      </c>
-      <c r="B8" s="21" t="n">
-        <v>12341234</v>
+      <c r="B8" s="20" t="s">
+        <v>291</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>289</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="20" t="s">
+        <v>293</v>
+      </c>
+      <c r="B9" s="20" t="s">
+        <v>294</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>289</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="20" t="s">
+        <v>295</v>
+      </c>
+      <c r="C10" s="20" t="s">
+        <v>289</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="20" t="s">
+        <v>296</v>
+      </c>
+      <c r="B11" s="20" t="n">
+        <v>587</v>
+      </c>
+      <c r="C11" s="20" t="s">
+        <v>289</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="20" t="s">
+        <v>297</v>
+      </c>
+      <c r="B12" s="20" t="s">
+        <v>298</v>
+      </c>
+      <c r="C12" s="20" t="s">
+        <v>289</v>
+      </c>
+      <c r="D12" s="20" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="20" t="s">
+        <v>299</v>
+      </c>
+      <c r="B13" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="C13" s="20" t="s">
+        <v>289</v>
+      </c>
+      <c r="D13" s="20" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="14.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="20" t="s">
+        <v>300</v>
+      </c>
+      <c r="B14" s="20" t="s">
+        <v>301</v>
+      </c>
+      <c r="C14" s="20" t="s">
+        <v>302</v>
+      </c>
+      <c r="D14" s="20" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="20" t="s">
+        <v>304</v>
+      </c>
+      <c r="B15" s="20" t="s">
+        <v>305</v>
+      </c>
+      <c r="C15" s="20" t="s">
+        <v>302</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B14" r:id="rId1" display="sparton.clinic1@gmail.com"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
added status to patient, changed seeds.rb to work with Upper/lower named tabs
</commit_message>
<xml_diff>
--- a/app1.xlsx
+++ b/app1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="8"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Status" sheetId="1" state="visible" r:id="rId2"/>
@@ -28,7 +28,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="306">
+  <si>
+    <t xml:space="preserve">id</t>
+  </si>
   <si>
     <t xml:space="preserve">status</t>
   </si>
@@ -36,6 +39,9 @@
     <t xml:space="preserve">description</t>
   </si>
   <si>
+    <t xml:space="preserve">integer</t>
+  </si>
+  <si>
     <t xml:space="preserve">string</t>
   </si>
   <si>
@@ -60,9 +66,6 @@
     <t xml:space="preserve">Permanently disabled from system</t>
   </si>
   <si>
-    <t xml:space="preserve">id</t>
-  </si>
-  <si>
     <t xml:space="preserve">name</t>
   </si>
   <si>
@@ -85,9 +88,6 @@
   </si>
   <si>
     <t xml:space="preserve">notes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">integer</t>
   </si>
   <si>
     <t xml:space="preserve">references</t>
@@ -952,13 +952,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="6">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="M/D/YYYY"/>
     <numFmt numFmtId="166" formatCode="MM/DD/YYYY"/>
     <numFmt numFmtId="167" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
     <numFmt numFmtId="168" formatCode="MM/DD/YYYY\ HH:MM:SS"/>
-    <numFmt numFmtId="169" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
   <fonts count="8">
     <font>
@@ -1152,7 +1151,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1234,17 +1233,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C39" activeCellId="0" sqref="C39"/>
+      <selection pane="topLeft" activeCell="E6" activeCellId="1" sqref="I1:I2 E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="9.91093117408907"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.2591093117409"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.91093117408907"/>
+    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="10.0404858299595"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.6234817813765"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="10.0404858299595"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1254,41 +1253,56 @@
       <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B4" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="1"/>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="1"/>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>8</v>
-      </c>
       <c r="B5" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="1"/>
+        <v>10</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1309,76 +1323,76 @@
   <dimension ref="A1:K65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I23" activeCellId="0" sqref="I23"/>
+      <selection pane="topLeft" activeCell="H1" activeCellId="1" sqref="I1:I2 H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="26.5668016194332"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="23.3805668016194"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="21.1821862348178"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="27.2995951417004"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="33.914979757085"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="24.8502024291498"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.54655870445344"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="27.2995951417004"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="23.8744939271255"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="21.5465587044534"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="27.9068825910931"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="34.6437246963563"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="25.4655870445344"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.66801619433198"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H2" s="0" t="s">
         <v>20</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1750,18 +1764,18 @@
   <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
+      <selection pane="topLeft" activeCell="A15" activeCellId="1" sqref="I1:I2 A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="24.1174089068826"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.91093117408907"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="24.7287449392713"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.0404858299595"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>97</v>
@@ -1772,10 +1786,10 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>99</v>
@@ -1791,7 +1805,7 @@
       </c>
       <c r="C3" s="1" t="n">
         <f aca="true">NOW() +RAND()*1000</f>
-        <v>42795.6802746477</v>
+        <v>43048.581132151</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1804,7 +1818,7 @@
       </c>
       <c r="C4" s="1" t="n">
         <f aca="true">NOW() +RAND()*1000</f>
-        <v>43057.3603312528</v>
+        <v>43445.6891394397</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1817,7 +1831,7 @@
       </c>
       <c r="C5" s="1" t="n">
         <f aca="true">NOW() +RAND()*1000</f>
-        <v>43127.9392892374</v>
+        <v>43050.773936856</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1830,7 +1844,7 @@
       </c>
       <c r="C6" s="1" t="n">
         <f aca="true">NOW() +RAND()*1000</f>
-        <v>43743.6417006672</v>
+        <v>42840.785055864</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1843,7 +1857,7 @@
       </c>
       <c r="C7" s="1" t="n">
         <f aca="true">NOW() +RAND()*1000</f>
-        <v>43130.3731738093</v>
+        <v>43585.0008007373</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1856,7 +1870,7 @@
       </c>
       <c r="C8" s="1" t="n">
         <f aca="true">NOW() +RAND()*1000</f>
-        <v>43240.2425823536</v>
+        <v>43085.5904669068</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1869,7 +1883,7 @@
       </c>
       <c r="C9" s="1" t="n">
         <f aca="true">NOW() +RAND()*1000</f>
-        <v>43214.0965490759</v>
+        <v>43704.8610797461</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1882,7 +1896,7 @@
       </c>
       <c r="C10" s="1" t="n">
         <f aca="true">NOW() +RAND()*1000</f>
-        <v>42807.2457316284</v>
+        <v>43315.6150769899</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1895,7 +1909,7 @@
       </c>
       <c r="C11" s="1" t="n">
         <f aca="true">NOW() +RAND()*1000</f>
-        <v>42829.0594259154</v>
+        <v>42849.2275733972</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1908,7 +1922,7 @@
       </c>
       <c r="C12" s="1" t="n">
         <f aca="true">NOW() +RAND()*1000</f>
-        <v>42960.7421623302</v>
+        <v>43321.261226226</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1921,7 +1935,7 @@
       </c>
       <c r="C13" s="1" t="n">
         <f aca="true">NOW() +RAND()*1000</f>
-        <v>43358.5612741858</v>
+        <v>43202.6481705545</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1934,7 +1948,7 @@
       </c>
       <c r="C14" s="1" t="n">
         <f aca="true">NOW() +RAND()*1000</f>
-        <v>42790.5915838549</v>
+        <v>43653.6824815256</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2177,22 +2191,22 @@
   <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
+      <selection pane="topLeft" activeCell="G4" activeCellId="1" sqref="I1:I2 G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="9.91093117408907"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.5222672064777"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.0364372469636"/>
-    <col collapsed="false" hidden="false" max="8" min="6" style="0" width="9.91093117408907"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="21.1821862348178"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="9.91093117408907"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="10.0404858299595"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23.0161943319838"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.5222672064777"/>
+    <col collapsed="false" hidden="false" max="8" min="6" style="0" width="10.0404858299595"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="21.5465587044534"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="10.0404858299595"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>100</v>
@@ -2232,13 +2246,13 @@
         <v>20</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>110</v>
@@ -2247,13 +2261,13 @@
         <v>110</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>99</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="K2" s="3"/>
       <c r="L2" s="4"/>
@@ -2280,11 +2294,11 @@
       </c>
       <c r="F3" s="3" t="n">
         <f aca="true">ROUND(RAND()*15+30,3)</f>
-        <v>33.964</v>
+        <v>40.851</v>
       </c>
       <c r="G3" s="3" t="n">
         <f aca="true">ROUND(-(RAND()*40+80),3)</f>
-        <v>-88.073</v>
+        <v>-112.302</v>
       </c>
       <c r="H3" s="3" t="str">
         <f aca="false">CONCATENATE(DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)))</f>
@@ -2292,7 +2306,7 @@
       </c>
       <c r="I3" s="5" t="n">
         <f aca="true">NOW()+100 + RAND()*365</f>
-        <v>42924.3640982918</v>
+        <v>43104.2525606538</v>
       </c>
       <c r="J3" s="3" t="n">
         <f aca="false">RANDBETWEEN(0,1000)</f>
@@ -2324,11 +2338,11 @@
       </c>
       <c r="F4" s="3" t="n">
         <f aca="true">ROUND(RAND()*15+30,3)</f>
-        <v>43.038</v>
+        <v>30.608</v>
       </c>
       <c r="G4" s="3" t="n">
         <f aca="true">ROUND(-(RAND()*40+80),3)</f>
-        <v>-104.373</v>
+        <v>-110.21</v>
       </c>
       <c r="H4" s="3" t="str">
         <f aca="false">CONCATENATE(DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)))</f>
@@ -2336,7 +2350,7 @@
       </c>
       <c r="I4" s="5" t="n">
         <f aca="true">NOW()+100 + RAND()*365</f>
-        <v>43188.0087600524</v>
+        <v>42981.9539025178</v>
       </c>
       <c r="J4" s="3" t="n">
         <f aca="false">RANDBETWEEN(0,1000)</f>
@@ -2368,11 +2382,11 @@
       </c>
       <c r="F5" s="3" t="n">
         <f aca="true">ROUND(RAND()*15+30,3)</f>
-        <v>37.474</v>
+        <v>43.522</v>
       </c>
       <c r="G5" s="3" t="n">
         <f aca="true">ROUND(-(RAND()*40+80),3)</f>
-        <v>-119.643</v>
+        <v>-84.987</v>
       </c>
       <c r="H5" s="3" t="str">
         <f aca="false">CONCATENATE(DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)))</f>
@@ -2380,7 +2394,7 @@
       </c>
       <c r="I5" s="5" t="n">
         <f aca="true">NOW()+100 + RAND()*365</f>
-        <v>42978.1741543979</v>
+        <v>42871.7280679418</v>
       </c>
       <c r="J5" s="3" t="n">
         <f aca="false">RANDBETWEEN(0,1000)</f>
@@ -2412,11 +2426,11 @@
       </c>
       <c r="F6" s="3" t="n">
         <f aca="true">ROUND(RAND()*15+30,3)</f>
-        <v>34.008</v>
+        <v>36.897</v>
       </c>
       <c r="G6" s="3" t="n">
         <f aca="true">ROUND(-(RAND()*40+80),3)</f>
-        <v>-82.049</v>
+        <v>-110.004</v>
       </c>
       <c r="H6" s="3" t="str">
         <f aca="false">CONCATENATE(DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)))</f>
@@ -2424,7 +2438,7 @@
       </c>
       <c r="I6" s="5" t="n">
         <f aca="true">NOW()+100 + RAND()*365</f>
-        <v>43016.7329581767</v>
+        <v>42860.7275607784</v>
       </c>
       <c r="J6" s="3" t="n">
         <f aca="false">RANDBETWEEN(0,1000)</f>
@@ -2456,11 +2470,11 @@
       </c>
       <c r="F7" s="3" t="n">
         <f aca="true">ROUND(RAND()*15+30,3)</f>
-        <v>42.887</v>
+        <v>31.781</v>
       </c>
       <c r="G7" s="3" t="n">
         <f aca="true">ROUND(-(RAND()*40+80),3)</f>
-        <v>-95.673</v>
+        <v>-104.332</v>
       </c>
       <c r="H7" s="3" t="str">
         <f aca="false">CONCATENATE(DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)))</f>
@@ -2468,7 +2482,7 @@
       </c>
       <c r="I7" s="5" t="n">
         <f aca="true">NOW()+100 + RAND()*365</f>
-        <v>43019.5173244928</v>
+        <v>43087.4364332775</v>
       </c>
       <c r="J7" s="3" t="n">
         <f aca="false">RANDBETWEEN(0,1000)</f>
@@ -2500,11 +2514,11 @@
       </c>
       <c r="F8" s="3" t="n">
         <f aca="true">ROUND(RAND()*15+30,3)</f>
-        <v>30.582</v>
+        <v>37.646</v>
       </c>
       <c r="G8" s="3" t="n">
         <f aca="true">ROUND(-(RAND()*40+80),3)</f>
-        <v>-119.424</v>
+        <v>-97.138</v>
       </c>
       <c r="H8" s="3" t="str">
         <f aca="false">CONCATENATE(DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)))</f>
@@ -2512,7 +2526,7 @@
       </c>
       <c r="I8" s="5" t="n">
         <f aca="true">NOW()+100 + RAND()*365</f>
-        <v>43135.3109004055</v>
+        <v>43151.4346376905</v>
       </c>
       <c r="J8" s="3" t="n">
         <f aca="false">RANDBETWEEN(0,1000)</f>
@@ -2544,11 +2558,11 @@
       </c>
       <c r="F9" s="3" t="n">
         <f aca="true">ROUND(RAND()*15+30,3)</f>
-        <v>39.814</v>
+        <v>44.317</v>
       </c>
       <c r="G9" s="3" t="n">
         <f aca="true">ROUND(-(RAND()*40+80),3)</f>
-        <v>-100.306</v>
+        <v>-85.405</v>
       </c>
       <c r="H9" s="3" t="str">
         <f aca="false">CONCATENATE(DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)))</f>
@@ -2556,7 +2570,7 @@
       </c>
       <c r="I9" s="5" t="n">
         <f aca="true">NOW()+100 + RAND()*365</f>
-        <v>43163.6342589653</v>
+        <v>42928.0496596545</v>
       </c>
       <c r="J9" s="3" t="n">
         <f aca="false">RANDBETWEEN(0,1000)</f>
@@ -2588,11 +2602,11 @@
       </c>
       <c r="F10" s="3" t="n">
         <f aca="true">ROUND(RAND()*15+30,3)</f>
-        <v>38.514</v>
+        <v>44.667</v>
       </c>
       <c r="G10" s="3" t="n">
         <f aca="true">ROUND(-(RAND()*40+80),3)</f>
-        <v>-104.27</v>
+        <v>-102.682</v>
       </c>
       <c r="H10" s="3" t="str">
         <f aca="false">CONCATENATE(DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)))</f>
@@ -2600,7 +2614,7 @@
       </c>
       <c r="I10" s="5" t="n">
         <f aca="true">NOW()+100 + RAND()*365</f>
-        <v>43042.154874953</v>
+        <v>42957.2747958365</v>
       </c>
       <c r="J10" s="3" t="n">
         <f aca="false">RANDBETWEEN(0,1000)</f>
@@ -2632,11 +2646,11 @@
       </c>
       <c r="F11" s="3" t="n">
         <f aca="true">ROUND(RAND()*15+30,3)</f>
-        <v>40.53</v>
+        <v>33.448</v>
       </c>
       <c r="G11" s="3" t="n">
         <f aca="true">ROUND(-(RAND()*40+80),3)</f>
-        <v>-103.404</v>
+        <v>-111.577</v>
       </c>
       <c r="H11" s="3" t="str">
         <f aca="false">CONCATENATE(DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)))</f>
@@ -2644,7 +2658,7 @@
       </c>
       <c r="I11" s="5" t="n">
         <f aca="true">NOW()+100 + RAND()*365</f>
-        <v>42885.675928022</v>
+        <v>43079.0344759285</v>
       </c>
       <c r="J11" s="3" t="n">
         <f aca="false">RANDBETWEEN(0,1000)</f>
@@ -2676,11 +2690,11 @@
       </c>
       <c r="F12" s="3" t="n">
         <f aca="true">ROUND(RAND()*15+30,3)</f>
-        <v>37.023</v>
+        <v>34.261</v>
       </c>
       <c r="G12" s="3" t="n">
         <f aca="true">ROUND(-(RAND()*40+80),3)</f>
-        <v>-82.759</v>
+        <v>-95.855</v>
       </c>
       <c r="H12" s="3" t="str">
         <f aca="false">CONCATENATE(DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)))</f>
@@ -2688,7 +2702,7 @@
       </c>
       <c r="I12" s="5" t="n">
         <f aca="true">NOW()+100 + RAND()*365</f>
-        <v>43196.2555472522</v>
+        <v>43062.8134901009</v>
       </c>
       <c r="J12" s="3" t="n">
         <f aca="false">RANDBETWEEN(0,1000)</f>
@@ -2720,11 +2734,11 @@
       </c>
       <c r="F13" s="3" t="n">
         <f aca="true">ROUND(RAND()*15+30,3)</f>
-        <v>43.096</v>
+        <v>44.821</v>
       </c>
       <c r="G13" s="3" t="n">
         <f aca="true">ROUND(-(RAND()*40+80),3)</f>
-        <v>-93.079</v>
+        <v>-83.194</v>
       </c>
       <c r="H13" s="3" t="str">
         <f aca="false">CONCATENATE(DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)))</f>
@@ -2732,7 +2746,7 @@
       </c>
       <c r="I13" s="5" t="n">
         <f aca="true">NOW()+100 + RAND()*365</f>
-        <v>42906.456119578</v>
+        <v>43075.129177402</v>
       </c>
       <c r="J13" s="3" t="n">
         <f aca="false">RANDBETWEEN(0,1000)</f>
@@ -2795,27 +2809,27 @@
   <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C27" activeCellId="0" sqref="C27"/>
+      <selection pane="topLeft" activeCell="C27" activeCellId="1" sqref="I1:I2 C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="6" width="9.91093117408907"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="6" width="26.4453441295547"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="6" width="12.2388663967611"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="6" width="9.91093117408907"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.5263157894737"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.91093117408907"/>
-    <col collapsed="false" hidden="false" max="12" min="7" style="6" width="17.2591093117409"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="9.91093117408907"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="6" width="10.0404858299595"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="6" width="27.0566801619433"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="6" width="12.4817813765182"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="6" width="10.0404858299595"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.6558704453441"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.0404858299595"/>
+    <col collapsed="false" hidden="false" max="12" min="7" style="6" width="17.6234817813765"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="10.0404858299595"/>
   </cols>
   <sheetData>
     <row r="1" s="8" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="7" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>100</v>
@@ -2850,22 +2864,22 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>20</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G2" s="10" t="s">
         <v>120</v>
@@ -4211,22 +4225,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1:I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="9.91093117408907"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.668016194332"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.91093117408907"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="10.0404858299595"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.919028340081"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.0404858299595"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>171</v>
@@ -4249,31 +4263,37 @@
       <c r="H1" s="0" t="s">
         <v>174</v>
       </c>
+      <c r="I1" s="0" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>99</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G2" s="0" t="s">
         <v>20</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4286,7 +4306,7 @@
       </c>
       <c r="C3" s="12" t="n">
         <f aca="true">NOW()-90*365*RAND()</f>
-        <v>39501.3414031615</v>
+        <v>12067.2374125906</v>
       </c>
       <c r="D3" s="0" t="s">
         <v>175</v>
@@ -4305,6 +4325,10 @@
         <f aca="false">CONCATENATE(E3, ".",F4,"@patient.com")</f>
         <v>Nathalia.Fisher@patient.com</v>
       </c>
+      <c r="I3" s="0" t="n">
+        <f aca="false">RANDBETWEEN(1,3)</f>
+        <v>3</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
@@ -4316,7 +4340,7 @@
       </c>
       <c r="C4" s="12" t="n">
         <f aca="true">NOW()-90*365*RAND()</f>
-        <v>16843.4421976712</v>
+        <v>41481.2958209769</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>175</v>
@@ -4335,6 +4359,10 @@
         <f aca="false">CONCATENATE(E4, ".",F5,"@patient.com")</f>
         <v>Grace.Bartlett@patient.com</v>
       </c>
+      <c r="I4" s="0" t="n">
+        <f aca="false">RANDBETWEEN(1,3)</f>
+        <v>3</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
@@ -4346,7 +4374,7 @@
       </c>
       <c r="C5" s="12" t="n">
         <f aca="true">NOW()-90*365*RAND()</f>
-        <v>21589.2368559503</v>
+        <v>18559.1907867494</v>
       </c>
       <c r="D5" s="0" t="s">
         <v>175</v>
@@ -4365,6 +4393,10 @@
         <f aca="false">CONCATENATE(E5, ".",F6,"@patient.com")</f>
         <v>Lucille.George@patient.com</v>
       </c>
+      <c r="I5" s="0" t="n">
+        <f aca="false">RANDBETWEEN(1,3)</f>
+        <v>3</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
@@ -4376,7 +4408,7 @@
       </c>
       <c r="C6" s="12" t="n">
         <f aca="true">NOW()-90*365*RAND()</f>
-        <v>40296.7035861034</v>
+        <v>41482.1488005623</v>
       </c>
       <c r="D6" s="0" t="s">
         <v>175</v>
@@ -4395,6 +4427,10 @@
         <f aca="false">CONCATENATE(E6, ".",F7,"@patient.com")</f>
         <v>Julianna.Hays@patient.com</v>
       </c>
+      <c r="I6" s="0" t="n">
+        <f aca="false">RANDBETWEEN(1,3)</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
@@ -4406,7 +4442,7 @@
       </c>
       <c r="C7" s="12" t="n">
         <f aca="true">NOW()-90*365*RAND()</f>
-        <v>39629.931569851</v>
+        <v>21762.1484677041</v>
       </c>
       <c r="D7" s="0" t="s">
         <v>175</v>
@@ -4425,6 +4461,10 @@
         <f aca="false">CONCATENATE(E7, ".",F8,"@patient.com")</f>
         <v>Lila.Mendoza@patient.com</v>
       </c>
+      <c r="I7" s="0" t="n">
+        <f aca="false">RANDBETWEEN(1,3)</f>
+        <v>3</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
@@ -4436,7 +4476,7 @@
       </c>
       <c r="C8" s="12" t="n">
         <f aca="true">NOW()-90*365*RAND()</f>
-        <v>31779.8979278321</v>
+        <v>35297.0771982089</v>
       </c>
       <c r="D8" s="0" t="s">
         <v>175</v>
@@ -4455,6 +4495,10 @@
         <f aca="false">CONCATENATE(E8, ".",F9,"@patient.com")</f>
         <v>Amina.Lindsey@patient.com</v>
       </c>
+      <c r="I8" s="0" t="n">
+        <f aca="false">RANDBETWEEN(1,3)</f>
+        <v>3</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
@@ -4466,7 +4510,7 @@
       </c>
       <c r="C9" s="12" t="n">
         <f aca="true">NOW()-90*365*RAND()</f>
-        <v>37302.381040631</v>
+        <v>23967.9354808073</v>
       </c>
       <c r="D9" s="0" t="s">
         <v>175</v>
@@ -4485,6 +4529,10 @@
         <f aca="false">CONCATENATE(E9, ".",F10,"@patient.com")</f>
         <v>Rachael.Case@patient.com</v>
       </c>
+      <c r="I9" s="0" t="n">
+        <f aca="false">RANDBETWEEN(1,3)</f>
+        <v>3</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
@@ -4496,7 +4544,7 @@
       </c>
       <c r="C10" s="12" t="n">
         <f aca="true">NOW()-90*365*RAND()</f>
-        <v>22902.0111697759</v>
+        <v>22157.1819320502</v>
       </c>
       <c r="D10" s="0" t="s">
         <v>175</v>
@@ -4515,6 +4563,10 @@
         <f aca="false">CONCATENATE(E10, ".",F11,"@patient.com")</f>
         <v>Harley.Ewing@patient.com</v>
       </c>
+      <c r="I10" s="0" t="n">
+        <f aca="false">RANDBETWEEN(1,3)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
@@ -4526,7 +4578,7 @@
       </c>
       <c r="C11" s="12" t="n">
         <f aca="true">NOW()-90*365*RAND()</f>
-        <v>35348.9109630396</v>
+        <v>15709.8315877116</v>
       </c>
       <c r="D11" s="0" t="s">
         <v>175</v>
@@ -4545,6 +4597,10 @@
         <f aca="false">CONCATENATE(E11, ".",F12,"@patient.com")</f>
         <v>Giuliana.Jefferson@patient.com</v>
       </c>
+      <c r="I11" s="0" t="n">
+        <f aca="false">RANDBETWEEN(1,3)</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
@@ -4556,7 +4612,7 @@
       </c>
       <c r="C12" s="12" t="n">
         <f aca="true">NOW()-90*365*RAND()</f>
-        <v>10753.9436332744</v>
+        <v>36391.4918161889</v>
       </c>
       <c r="D12" s="0" t="s">
         <v>175</v>
@@ -4575,6 +4631,10 @@
         <f aca="false">CONCATENATE(E12, ".",F13,"@patient.com")</f>
         <v>Ariella.Dickson@patient.com</v>
       </c>
+      <c r="I12" s="0" t="n">
+        <f aca="false">RANDBETWEEN(1,3)</f>
+        <v>3</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
@@ -4586,7 +4646,7 @@
       </c>
       <c r="C13" s="12" t="n">
         <f aca="true">NOW()-90*365*RAND()</f>
-        <v>31957.2587588869</v>
+        <v>26328.7723035705</v>
       </c>
       <c r="D13" s="0" t="s">
         <v>175</v>
@@ -4605,6 +4665,10 @@
         <f aca="false">CONCATENATE(E13, ".",F14,"@patient.com")</f>
         <v>Nelson.Serrano@patient.com</v>
       </c>
+      <c r="I13" s="0" t="n">
+        <f aca="false">RANDBETWEEN(1,3)</f>
+        <v>3</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
@@ -4616,7 +4680,7 @@
       </c>
       <c r="C14" s="12" t="n">
         <f aca="true">NOW()-90*365*RAND()</f>
-        <v>21104.7958335609</v>
+        <v>18672.3033227309</v>
       </c>
       <c r="D14" s="0" t="s">
         <v>196</v>
@@ -4635,6 +4699,10 @@
         <f aca="false">CONCATENATE(E14, ".",F15,"@patient.com")</f>
         <v>Brennan.Morton@patient.com</v>
       </c>
+      <c r="I14" s="0" t="n">
+        <f aca="false">RANDBETWEEN(1,3)</f>
+        <v>3</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
@@ -4646,7 +4714,7 @@
       </c>
       <c r="C15" s="12" t="n">
         <f aca="true">NOW()-90*365*RAND()</f>
-        <v>11527.5258166523</v>
+        <v>32295.5620953713</v>
       </c>
       <c r="D15" s="0" t="s">
         <v>196</v>
@@ -4665,6 +4733,10 @@
         <f aca="false">CONCATENATE(E15, ".",F16,"@patient.com")</f>
         <v>Colt.Foley@patient.com</v>
       </c>
+      <c r="I15" s="0" t="n">
+        <f aca="false">RANDBETWEEN(1,3)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
@@ -4676,7 +4748,7 @@
       </c>
       <c r="C16" s="12" t="n">
         <f aca="true">NOW()-90*365*RAND()</f>
-        <v>11655.6557118445</v>
+        <v>37528.1457867249</v>
       </c>
       <c r="D16" s="0" t="s">
         <v>196</v>
@@ -4695,6 +4767,10 @@
         <f aca="false">CONCATENATE(E16, ".",F17,"@patient.com")</f>
         <v>Dax.Benson@patient.com</v>
       </c>
+      <c r="I16" s="0" t="n">
+        <f aca="false">RANDBETWEEN(1,3)</f>
+        <v>3</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
@@ -4706,7 +4782,7 @@
       </c>
       <c r="C17" s="12" t="n">
         <f aca="true">NOW()-90*365*RAND()</f>
-        <v>28414.3802652895</v>
+        <v>19450.9324562136</v>
       </c>
       <c r="D17" s="0" t="s">
         <v>196</v>
@@ -4725,6 +4801,10 @@
         <f aca="false">CONCATENATE(E17, ".",F18,"@patient.com")</f>
         <v>Dominic.Maldonado@patient.com</v>
       </c>
+      <c r="I17" s="0" t="n">
+        <f aca="false">RANDBETWEEN(1,3)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
@@ -4736,7 +4816,7 @@
       </c>
       <c r="C18" s="12" t="n">
         <f aca="true">NOW()-90*365*RAND()</f>
-        <v>29591.977886474</v>
+        <v>14874.9902891343</v>
       </c>
       <c r="D18" s="0" t="s">
         <v>196</v>
@@ -4755,6 +4835,10 @@
         <f aca="false">CONCATENATE(E18, ".",F19,"@patient.com")</f>
         <v>Matteo.Schmitt@patient.com</v>
       </c>
+      <c r="I18" s="0" t="n">
+        <f aca="false">RANDBETWEEN(1,3)</f>
+        <v>3</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
@@ -4766,7 +4850,7 @@
       </c>
       <c r="C19" s="12" t="n">
         <f aca="true">NOW()-90*365*RAND()</f>
-        <v>33342.0815425449</v>
+        <v>16021.4500940599</v>
       </c>
       <c r="D19" s="0" t="s">
         <v>196</v>
@@ -4785,6 +4869,10 @@
         <f aca="false">CONCATENATE(E19, ".",F20,"@patient.com")</f>
         <v>Augustus.Greer@patient.com</v>
       </c>
+      <c r="I19" s="0" t="n">
+        <f aca="false">RANDBETWEEN(1,3)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
@@ -4796,7 +4884,7 @@
       </c>
       <c r="C20" s="12" t="n">
         <f aca="true">NOW()-90*365*RAND()</f>
-        <v>36508.8843419367</v>
+        <v>10907.6500887383</v>
       </c>
       <c r="D20" s="0" t="s">
         <v>196</v>
@@ -4815,6 +4903,10 @@
         <f aca="false">CONCATENATE(E20, ".",F21,"@patient.com")</f>
         <v>Nathen.Pierce@patient.com</v>
       </c>
+      <c r="I20" s="0" t="n">
+        <f aca="false">RANDBETWEEN(1,3)</f>
+        <v>3</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
@@ -4826,7 +4918,7 @@
       </c>
       <c r="C21" s="12" t="n">
         <f aca="true">NOW()-90*365*RAND()</f>
-        <v>26560.5731057971</v>
+        <v>12457.2119495394</v>
       </c>
       <c r="D21" s="0" t="s">
         <v>196</v>
@@ -4845,6 +4937,10 @@
         <f aca="false">CONCATENATE(E21, ".",F22,"@patient.com")</f>
         <v>Jordan.Dodson@patient.com</v>
       </c>
+      <c r="I21" s="0" t="n">
+        <f aca="false">RANDBETWEEN(1,3)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
@@ -4856,7 +4952,7 @@
       </c>
       <c r="C22" s="12" t="n">
         <f aca="true">NOW()-90*365*RAND()</f>
-        <v>16116.583948489</v>
+        <v>15521.9308839509</v>
       </c>
       <c r="D22" s="0" t="s">
         <v>196</v>
@@ -4874,6 +4970,10 @@
       <c r="H22" s="0" t="str">
         <f aca="false">CONCATENATE(E22, ".",F23,"@patient.com")</f>
         <v>Agustin.@patient.com</v>
+      </c>
+      <c r="I22" s="0" t="n">
+        <f aca="false">RANDBETWEEN(1,3)</f>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -4895,20 +4995,20 @@
   <dimension ref="A1:M35"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A36" activeCellId="0" sqref="A36"/>
+      <selection pane="topLeft" activeCell="A36" activeCellId="1" sqref="I1:I2 A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="7" min="1" style="6" width="9.78947368421053"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="13" width="24.3603238866397"/>
-    <col collapsed="false" hidden="false" max="13" min="9" style="0" width="24.3603238866397"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="9.91093117408907"/>
+    <col collapsed="false" hidden="false" max="7" min="1" style="6" width="9.91093117408907"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="13" width="24.9716599190283"/>
+    <col collapsed="false" hidden="false" max="13" min="9" style="0" width="24.9716599190283"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="10.0404858299595"/>
   </cols>
   <sheetData>
     <row r="1" s="16" customFormat="true" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="14" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>215</v>
@@ -4932,12 +5032,12 @@
         <v>220</v>
       </c>
       <c r="I1" s="16" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>20</v>
@@ -4961,7 +5061,7 @@
         <v>221</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4994,7 +5094,7 @@
       </c>
       <c r="H3" s="17" t="n">
         <f aca="true">NOW() -RAND()*99.7</f>
-        <v>42743.1902499568</v>
+        <v>42686.2818895909</v>
       </c>
       <c r="I3" s="0" t="s">
         <v>222</v>
@@ -5030,7 +5130,7 @@
       </c>
       <c r="H4" s="17" t="n">
         <f aca="true">NOW() -RAND()*100</f>
-        <v>42736.3535385482</v>
+        <v>42719.7839805644</v>
       </c>
       <c r="I4" s="0" t="s">
         <v>223</v>
@@ -5068,7 +5168,7 @@
       </c>
       <c r="H5" s="17" t="n">
         <f aca="true">NOW() -RAND()*100</f>
-        <v>42709.4845487654</v>
+        <v>42699.9558453535</v>
       </c>
       <c r="I5" s="0" t="s">
         <v>224</v>
@@ -5106,7 +5206,7 @@
       </c>
       <c r="H6" s="17" t="n">
         <f aca="true">NOW() -RAND()*100</f>
-        <v>42672.3532023695</v>
+        <v>42667.7116706716</v>
       </c>
       <c r="I6" s="0" t="s">
         <v>225</v>
@@ -5144,7 +5244,7 @@
       </c>
       <c r="H7" s="17" t="n">
         <f aca="true">NOW() -RAND()*100</f>
-        <v>42745.8495281464</v>
+        <v>42727.1738036959</v>
       </c>
       <c r="I7" s="0" t="s">
         <v>226</v>
@@ -5182,7 +5282,7 @@
       </c>
       <c r="H8" s="17" t="n">
         <f aca="true">NOW() -RAND()*100</f>
-        <v>42700.3469847428</v>
+        <v>42661.4644856743</v>
       </c>
       <c r="I8" s="0" t="s">
         <v>227</v>
@@ -5220,7 +5320,7 @@
       </c>
       <c r="H9" s="17" t="n">
         <f aca="true">NOW() -RAND()*100</f>
-        <v>42745.7254026287</v>
+        <v>42669.4810108935</v>
       </c>
       <c r="I9" s="0" t="s">
         <v>228</v>
@@ -5258,7 +5358,7 @@
       </c>
       <c r="H10" s="17" t="n">
         <f aca="true">NOW() -RAND()*100</f>
-        <v>42665.0375584331</v>
+        <v>42724.1119924583</v>
       </c>
       <c r="I10" s="0" t="s">
         <v>229</v>
@@ -5296,7 +5396,7 @@
       </c>
       <c r="H11" s="17" t="n">
         <f aca="true">NOW() -RAND()*100</f>
-        <v>42740.6957093297</v>
+        <v>42673.9741394464</v>
       </c>
       <c r="I11" s="0" t="s">
         <v>230</v>
@@ -5334,7 +5434,7 @@
       </c>
       <c r="H12" s="17" t="n">
         <f aca="true">NOW() -RAND()*100</f>
-        <v>42737.9709746287</v>
+        <v>42664.523919602</v>
       </c>
       <c r="I12" s="0" t="s">
         <v>231</v>
@@ -5372,7 +5472,7 @@
       </c>
       <c r="H13" s="17" t="n">
         <f aca="true">NOW() -RAND()*100</f>
-        <v>42710.0690547679</v>
+        <v>42746.0149152288</v>
       </c>
       <c r="I13" s="0" t="s">
         <v>232</v>
@@ -5410,7 +5510,7 @@
       </c>
       <c r="H14" s="17" t="n">
         <f aca="true">NOW() -RAND()*100</f>
-        <v>42716.0171368997</v>
+        <v>42745.789357431</v>
       </c>
       <c r="I14" s="0" t="s">
         <v>233</v>
@@ -5448,7 +5548,7 @@
       </c>
       <c r="H15" s="17" t="n">
         <f aca="true">NOW() -RAND()*100</f>
-        <v>42674.7783471665</v>
+        <v>42701.68788953</v>
       </c>
       <c r="I15" s="0" t="s">
         <v>234</v>
@@ -5486,7 +5586,7 @@
       </c>
       <c r="H16" s="17" t="n">
         <f aca="true">NOW() -RAND()*100</f>
-        <v>42722.8316821317</v>
+        <v>42731.4236765044</v>
       </c>
       <c r="I16" s="0" t="s">
         <v>235</v>
@@ -5524,7 +5624,7 @@
       </c>
       <c r="H17" s="17" t="n">
         <f aca="true">NOW() -RAND()*100</f>
-        <v>42757.1599649736</v>
+        <v>42687.8129334642</v>
       </c>
       <c r="I17" s="0" t="s">
         <v>236</v>
@@ -5562,7 +5662,7 @@
       </c>
       <c r="H18" s="17" t="n">
         <f aca="true">NOW() -RAND()*100</f>
-        <v>42679.0609330361</v>
+        <v>42715.4976293328</v>
       </c>
       <c r="I18" s="0" t="s">
         <v>237</v>
@@ -5600,7 +5700,7 @@
       </c>
       <c r="H19" s="17" t="n">
         <f aca="true">NOW() -RAND()*100</f>
-        <v>42674.6825612462</v>
+        <v>42679.1378471485</v>
       </c>
       <c r="I19" s="0" t="s">
         <v>238</v>
@@ -5638,7 +5738,7 @@
       </c>
       <c r="H20" s="17" t="n">
         <f aca="true">NOW() -RAND()*100</f>
-        <v>42731.8205698679</v>
+        <v>42733.8892080376</v>
       </c>
       <c r="I20" s="0" t="s">
         <v>239</v>
@@ -5676,7 +5776,7 @@
       </c>
       <c r="H21" s="17" t="n">
         <f aca="true">NOW() -RAND()*100</f>
-        <v>42696.5219224288</v>
+        <v>42670.5338887399</v>
       </c>
       <c r="I21" s="0" t="s">
         <v>240</v>
@@ -5714,7 +5814,7 @@
       </c>
       <c r="H22" s="17" t="n">
         <f aca="true">NOW() -RAND()*100</f>
-        <v>42682.4390475461</v>
+        <v>42699.1529789212</v>
       </c>
       <c r="I22" s="0" t="s">
         <v>241</v>
@@ -5752,7 +5852,7 @@
       </c>
       <c r="H23" s="17" t="n">
         <f aca="true">NOW() -RAND()*100</f>
-        <v>42700.7478095004</v>
+        <v>42682.6662165088</v>
       </c>
       <c r="I23" s="0" t="s">
         <v>242</v>
@@ -5790,7 +5890,7 @@
       </c>
       <c r="H24" s="17" t="n">
         <f aca="true">NOW() -RAND()*100</f>
-        <v>42687.6765431392</v>
+        <v>42681.3249704936</v>
       </c>
       <c r="I24" s="0" t="s">
         <v>243</v>
@@ -5828,7 +5928,7 @@
       </c>
       <c r="H25" s="17" t="n">
         <f aca="true">NOW() -RAND()*100</f>
-        <v>42740.2206678902</v>
+        <v>42676.812518584</v>
       </c>
       <c r="I25" s="0" t="s">
         <v>244</v>
@@ -5866,7 +5966,7 @@
       </c>
       <c r="H26" s="17" t="n">
         <f aca="true">NOW() -RAND()*100</f>
-        <v>42738.5250510615</v>
+        <v>42734.9284760234</v>
       </c>
       <c r="I26" s="0" t="s">
         <v>245</v>
@@ -5904,7 +6004,7 @@
       </c>
       <c r="H27" s="17" t="n">
         <f aca="true">NOW() -RAND()*100</f>
-        <v>42760.6308758008</v>
+        <v>42691.3076614938</v>
       </c>
       <c r="I27" s="0" t="s">
         <v>246</v>
@@ -5942,7 +6042,7 @@
       </c>
       <c r="H28" s="17" t="n">
         <f aca="true">NOW() -RAND()*100</f>
-        <v>42710.4316849075</v>
+        <v>42753.6685457181</v>
       </c>
       <c r="I28" s="0" t="s">
         <v>247</v>
@@ -5980,7 +6080,7 @@
       </c>
       <c r="H29" s="17" t="n">
         <f aca="true">NOW() -RAND()*100</f>
-        <v>42749.0461795868</v>
+        <v>42728.8512368799</v>
       </c>
       <c r="I29" s="0" t="s">
         <v>248</v>
@@ -6018,7 +6118,7 @@
       </c>
       <c r="H30" s="17" t="n">
         <f aca="true">NOW() -RAND()*100</f>
-        <v>42674.0564125614</v>
+        <v>42730.0392224162</v>
       </c>
       <c r="I30" s="0" t="s">
         <v>249</v>
@@ -6056,7 +6156,7 @@
       </c>
       <c r="H31" s="17" t="n">
         <f aca="true">NOW() -RAND()*100</f>
-        <v>42689.4790010351</v>
+        <v>42747.394324689</v>
       </c>
       <c r="I31" s="0" t="s">
         <v>250</v>
@@ -6094,7 +6194,7 @@
       </c>
       <c r="H32" s="17" t="n">
         <f aca="true">NOW() -RAND()*100</f>
-        <v>42664.8385308753</v>
+        <v>42666.2649731001</v>
       </c>
       <c r="I32" s="0" t="s">
         <v>251</v>
@@ -6132,7 +6232,7 @@
       </c>
       <c r="H33" s="17" t="n">
         <f aca="true">NOW() -RAND()*100</f>
-        <v>42701.7328191303</v>
+        <v>42693.4368826213</v>
       </c>
       <c r="I33" s="0" t="s">
         <v>252</v>
@@ -6170,7 +6270,7 @@
       </c>
       <c r="H34" s="17" t="n">
         <f aca="true">NOW() -RAND()*100</f>
-        <v>42677.9292542771</v>
+        <v>42743.6857672072</v>
       </c>
       <c r="I34" s="0" t="s">
         <v>253</v>
@@ -6208,7 +6308,7 @@
       </c>
       <c r="H35" s="17" t="n">
         <f aca="true">NOW() -RAND()*100</f>
-        <v>42735.8974739042</v>
+        <v>42692.4662221979</v>
       </c>
       <c r="I35" s="0" t="s">
         <v>254</v>
@@ -6235,16 +6335,16 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
+      <selection pane="topLeft" activeCell="A18" activeCellId="1" sqref="I1:I2 A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="18" width="31.7085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="18" width="14.3238866396761"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="18" width="28.7732793522267"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="18" width="11.3846153846154"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="18" width="9.30364372469636"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="18" width="32.4412955465587"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="18" width="14.6882591093117"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="18" width="29.3805668016194"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="18" width="11.6315789473684"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="18" width="9.4251012145749"/>
   </cols>
   <sheetData>
     <row r="1" s="19" customFormat="true" ht="14.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6427,18 +6527,18 @@
   </sheetPr>
   <dimension ref="1:15"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D18" activeCellId="1" sqref="I1:I2 D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="20" width="21.7935222672065"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="20" width="32.6275303643725"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="20" width="34.3765182186235"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="20" width="57.7813765182186"/>
-    <col collapsed="false" hidden="false" max="1023" min="5" style="20" width="9.30364372469636"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="9.30364372469636"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="20" width="22.2793522267206"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="20" width="33.4210526315789"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="20" width="35.1336032388664"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="20" width="59.1295546558704"/>
+    <col collapsed="false" hidden="false" max="1023" min="5" style="20" width="9.4251012145749"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="9.4251012145749"/>
   </cols>
   <sheetData>
     <row r="1" s="21" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6570,7 +6670,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="20" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B10" s="20" t="s">
         <v>295</v>
@@ -6614,7 +6714,8 @@
       <c r="A13" s="20" t="s">
         <v>299</v>
       </c>
-      <c r="B13" s="23" t="b">
+      <c r="B13" s="23" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C13" s="20" t="s">

</xml_diff>